<commit_message>
Clean nav-data and update helsedirektoratet
</commit_message>
<xml_diff>
--- a/data/02_admissions/admissions.xlsx
+++ b/data/02_admissions/admissions.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C653"/>
+  <dimension ref="A1:C676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8857,6 +8857,305 @@
         <v>31</v>
       </c>
     </row>
+    <row r="654">
+      <c r="A654" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Akershus universitetssykehus HF</t>
+        </is>
+      </c>
+      <c r="C654">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Diakonhjemmet Sykehus</t>
+        </is>
+      </c>
+      <c r="C655">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Finnmarkssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C656">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Haraldsplass Diakonale Sykehus</t>
+        </is>
+      </c>
+      <c r="C657">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Helgelandssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C658">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Helse Bergen HF</t>
+        </is>
+      </c>
+      <c r="C659">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Helse Fonna HF</t>
+        </is>
+      </c>
+      <c r="C660">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Helse Førde HF</t>
+        </is>
+      </c>
+      <c r="C661">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Helse Møre og Romsdal</t>
+        </is>
+      </c>
+      <c r="C662">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Helse Nord-Trøndelag</t>
+        </is>
+      </c>
+      <c r="C663">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Helse Stavanger HF</t>
+        </is>
+      </c>
+      <c r="C664">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Lovisenberg Diakonale Sykehus</t>
+        </is>
+      </c>
+      <c r="C665">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Nordlandssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C666">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Oslo universitetssykehus HF</t>
+        </is>
+      </c>
+      <c r="C667">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Sørlandet sykehus HF</t>
+        </is>
+      </c>
+      <c r="C668">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>St. Olavs hospital</t>
+        </is>
+      </c>
+      <c r="C669">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Sunnaas sykehus HF</t>
+        </is>
+      </c>
+      <c r="C670">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Sykehuset Innlandet HF</t>
+        </is>
+      </c>
+      <c r="C671">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Sykehuset i Vestfold HF</t>
+        </is>
+      </c>
+      <c r="C672">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Sykehuset Østfold HF</t>
+        </is>
+      </c>
+      <c r="C673">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Sykehuset Telemark HF</t>
+        </is>
+      </c>
+      <c r="C674">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Universitetssykehuset Nord-Norge HF</t>
+        </is>
+      </c>
+      <c r="C675">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Vestre Viken HF</t>
+        </is>
+      </c>
+      <c r="C676">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload code-folder and update all files
</commit_message>
<xml_diff>
--- a/data/02_admissions/admissions.xlsx
+++ b/data/02_admissions/admissions.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C806"/>
+  <dimension ref="A1:C829"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10846,6 +10846,305 @@
         <v>20</v>
       </c>
     </row>
+    <row r="807">
+      <c r="A807" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Akershus universitetssykehus HF</t>
+        </is>
+      </c>
+      <c r="C807">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Diakonhjemmet Sykehus</t>
+        </is>
+      </c>
+      <c r="C808">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Finnmarkssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C809">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Haraldsplass Diakonale Sykehus</t>
+        </is>
+      </c>
+      <c r="C810">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Helgelandssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C811">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Helse Bergen HF</t>
+        </is>
+      </c>
+      <c r="C812">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Helse Fonna HF</t>
+        </is>
+      </c>
+      <c r="C813">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Helse Førde HF</t>
+        </is>
+      </c>
+      <c r="C814">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Helse Møre og Romsdal</t>
+        </is>
+      </c>
+      <c r="C815">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Helse Nord-Trøndelag</t>
+        </is>
+      </c>
+      <c r="C816">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Helse Stavanger HF</t>
+        </is>
+      </c>
+      <c r="C817">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Lovisenberg Diakonale Sykehus</t>
+        </is>
+      </c>
+      <c r="C818">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Nordlandssykehuset HF</t>
+        </is>
+      </c>
+      <c r="C819">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Oslo universitetssykehus HF</t>
+        </is>
+      </c>
+      <c r="C820">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Sørlandet sykehus HF</t>
+        </is>
+      </c>
+      <c r="C821">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>St. Olavs hospital</t>
+        </is>
+      </c>
+      <c r="C822">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Sunnaas Sykehus HF</t>
+        </is>
+      </c>
+      <c r="C823">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Sykehuset Innlandet HF</t>
+        </is>
+      </c>
+      <c r="C824">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Sykehuset i Vestfold HF</t>
+        </is>
+      </c>
+      <c r="C825">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Sykehuset Østfold HF</t>
+        </is>
+      </c>
+      <c r="C826">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Sykehuset Telemark HF</t>
+        </is>
+      </c>
+      <c r="C827">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Universitetssykehuset Nord-Norge HF</t>
+        </is>
+      </c>
+      <c r="C828">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Vestre Viken HF</t>
+        </is>
+      </c>
+      <c r="C829">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>